<commit_message>
adding bootstrap curve sheet
</commit_message>
<xml_diff>
--- a/XL_pricer/CDSCurve/CDSCurve_BBG.xlsx
+++ b/XL_pricer/CDSCurve/CDSCurve_BBG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dpsugasa\WorkFiles\deriv_models\High Yield Bond\highyieldbond\XL_pricer\CDSCurve\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BBAB9E8-4896-4158-BD9C-0C4B79BB0A83}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3355C555-8841-466D-9CE4-E1C246AE64DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="10980" tabRatio="230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="sub_recovery">#REF!</definedName>
     <definedName name="Today">EONIA!$C$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1238,13 +1238,22 @@
   <volType type="realTimeData">
     <main first="bloomberg.rtd">
       <tp>
-        <v>136.1</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188948 CMAN Curncy</stp>
-        <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R10C7</stp>
-        <tr r="G10" s="6"/>
+        <v>0.4</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188936 CMAN Curncy</stp>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R8C8</stp>
+        <tr r="H8" s="6"/>
+      </tp>
+      <tp>
+        <v>0.4</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188942 CMAN Curncy</stp>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R9C8</stp>
+        <tr r="H9" s="6"/>
       </tp>
       <tp>
         <v>161.46999999999997</v>
@@ -1252,47 +1261,11 @@
         <stp>##V3_BDPV12</stp>
         <stp>CY188954 CMAN Curncy</stp>
         <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R11C7</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R11C7</stp>
         <tr r="G11" s="6"/>
       </tp>
-      <tp t="s">
-        <v>GALP PL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188942 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R9C3</stp>
-        <tr r="C9" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.27529999999999999</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWE2F  CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[EoniaOIS_BBG.xlsx]EONIA!R18C6</stp>
-        <tr r="F18" s="2"/>
-      </tp>
-      <tp>
-        <v>-0.36099999999999999</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWE2Z  CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R3C6</stp>
-        <tr r="F3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>GALP PL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188918 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R5C3</stp>
-        <tr r="C5" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.2382</v>
+      <tp>
+        <v>-0.24249999999999999</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE3   CMPN Curncy</stp>
@@ -1301,7 +1274,7 @@
         <tr r="F19" s="2"/>
       </tp>
       <tp>
-        <v>0.78100000000000003</v>
+        <v>0.77800000000000002</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE15  CMPN Curncy</stp>
@@ -1309,26 +1282,17 @@
         <stp>[CDSCurve_BBG.xlsx]EONIA!R29C6</stp>
         <tr r="F29" s="2"/>
       </tp>
-      <tp t="s">
-        <v>GALP PL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188948 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R10C3</stp>
-        <tr r="C10" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>GALP PL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188936 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R8C3</stp>
-        <tr r="C8" s="6"/>
-      </tp>
-      <tp>
-        <v>0.58750000000000002</v>
+      <tp>
+        <v>-0.27900000000000003</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWE2F  CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R18C6</stp>
+        <tr r="F18" s="2"/>
+      </tp>
+      <tp>
+        <v>0.58399999999999996</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE12  CMPN Curncy</stp>
@@ -1336,17 +1300,26 @@
         <stp>[CDSCurve_BBG.xlsx]EONIA!R28C6</stp>
         <tr r="F28" s="2"/>
       </tp>
-      <tp t="s">
-        <v>GALP PL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188954 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R11C3</stp>
-        <tr r="C11" s="6"/>
-      </tp>
-      <tp>
-        <v>0.50349999999999995</v>
+      <tp>
+        <v>136.1</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188948 CMAN Curncy</stp>
+        <stp>CDS_FLAT_SPREAD</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R10C7</stp>
+        <tr r="G10" s="6"/>
+      </tp>
+      <tp>
+        <v>-0.31069999999999998</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWE2   CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R17C6</stp>
+        <tr r="F17" s="2"/>
+      </tp>
+      <tp>
+        <v>0.50270000000000004</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE11  CMPN Curncy</stp>
@@ -1355,7 +1328,16 @@
         <tr r="F27" s="2"/>
       </tp>
       <tp>
-        <v>0.41549999999999998</v>
+        <v>-0.33639999999999998</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWE1F  CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R16C6</stp>
+        <tr r="F16" s="2"/>
+      </tp>
+      <tp>
+        <v>0.4133</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE10  CMPN Curncy</stp>
@@ -1364,7 +1346,7 @@
         <tr r="F26" s="2"/>
       </tp>
       <tp>
-        <v>0.32069999999999999</v>
+        <v>0.32019999999999998</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE9   CMPN Curncy</stp>
@@ -1373,7 +1355,7 @@
         <tr r="F25" s="2"/>
       </tp>
       <tp>
-        <v>1.0615000000000001</v>
+        <v>1.0618000000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE50  CMPN Curncy</stp>
@@ -1381,17 +1363,17 @@
         <stp>[CDSCurve_BBG.xlsx]EONIA!R35C6</stp>
         <tr r="F35" s="2"/>
       </tp>
-      <tp t="s">
-        <v>GALP PL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188924 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R6C3</stp>
-        <tr r="C6" s="6"/>
-      </tp>
-      <tp>
-        <v>0.2225</v>
+      <tp>
+        <v>-0.35199999999999998</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWE1   CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R15C6</stp>
+        <tr r="F15" s="2"/>
+      </tp>
+      <tp>
+        <v>0.2208</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE8   CMPN Curncy</stp>
@@ -1400,7 +1382,7 @@
         <tr r="F24" s="2"/>
       </tp>
       <tp>
-        <v>1.0694999999999999</v>
+        <v>1.0708</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE40  CMPN Curncy</stp>
@@ -1409,7 +1391,16 @@
         <tr r="F34" s="2"/>
       </tp>
       <tp>
-        <v>0.123</v>
+        <v>-0.35349999999999998</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWEK   CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R14C6</stp>
+        <tr r="F14" s="2"/>
+      </tp>
+      <tp>
+        <v>0.1205</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE7   CMPN Curncy</stp>
@@ -1418,7 +1409,7 @@
         <tr r="F23" s="2"/>
       </tp>
       <tp>
-        <v>1.0697000000000001</v>
+        <v>1.0689</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE35  CMPN Curncy</stp>
@@ -1427,7 +1418,25 @@
         <tr r="F33" s="2"/>
       </tp>
       <tp>
-        <v>2.5700000000000001E-2</v>
+        <v>-0.35499999999999998</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWEJ   CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R13C6</stp>
+        <tr r="F13" s="2"/>
+      </tp>
+      <tp>
+        <v>0.4</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188924 CMAN Curncy</stp>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R6C8</stp>
+        <tr r="H6" s="6"/>
+      </tp>
+      <tp>
+        <v>2.1499999999999998E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE6   CMPN Curncy</stp>
@@ -1436,7 +1445,7 @@
         <tr r="F22" s="2"/>
       </tp>
       <tp>
-        <v>1.0629999999999999</v>
+        <v>1.0625</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE30  CMPN Curncy</stp>
@@ -1445,7 +1454,7 @@
         <tr r="F32" s="2"/>
       </tp>
       <tp>
-        <v>-0.35570000000000002</v>
+        <v>-0.35699999999999998</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWEI   CMPN Curncy</stp>
@@ -1454,7 +1463,16 @@
         <tr r="F12" s="2"/>
       </tp>
       <tp>
-        <v>-7.0499999999999993E-2</v>
+        <v>0.4</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188930 CMAN Curncy</stp>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R7C8</stp>
+        <tr r="H7" s="6"/>
+      </tp>
+      <tp>
+        <v>-7.2999999999999995E-2</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE5   CMPN Curncy</stp>
@@ -1463,7 +1481,7 @@
         <tr r="F21" s="2"/>
       </tp>
       <tp>
-        <v>1.0347</v>
+        <v>1.0335000000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE25  CMPN Curncy</stp>
@@ -1471,17 +1489,26 @@
         <stp>[CDSCurve_BBG.xlsx]EONIA!R31C6</stp>
         <tr r="F31" s="2"/>
       </tp>
-      <tp t="s">
-        <v>GALP PL</v>
+      <tp>
+        <v>-0.35799999999999998</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWEH   CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R11C6</stp>
+        <tr r="F11" s="2"/>
+      </tp>
+      <tp>
+        <v>0.4</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>CY188912 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R4C3</stp>
-        <tr r="C4" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.1578</v>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R4C8</stp>
+        <tr r="H4" s="6"/>
+      </tp>
+      <tp>
+        <v>-0.1605</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE4   CMPN Curncy</stp>
@@ -1490,7 +1517,7 @@
         <tr r="F20" s="2"/>
       </tp>
       <tp>
-        <v>0.96250000000000002</v>
+        <v>0.96120000000000005</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWE20  CMPN Curncy</stp>
@@ -1498,122 +1525,34 @@
         <stp>[CDSCurve_BBG.xlsx]EONIA!R30C6</stp>
         <tr r="F30" s="2"/>
       </tp>
-      <tp t="s">
-        <v>GALP PL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188930 CMAN Curncy</stp>
-        <stp>PRIMARY_EQUITY_TICKER</stp>
-        <stp>[CDS.xlsx]CDSCurve!R7C3</stp>
-        <tr r="C7" s="6"/>
-      </tp>
-      <tp>
-        <v>3</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188930 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R7C6</stp>
-        <tr r="F7" s="6"/>
-      </tp>
-      <tp>
-        <v>0.5</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188912 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R4C6</stp>
-        <tr r="F4" s="6"/>
-      </tp>
-      <tp>
-        <v>10</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188954 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R11C6</stp>
-        <tr r="F11" s="6"/>
-      </tp>
-      <tp>
-        <v>7</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188948 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R10C6</stp>
-        <tr r="F10" s="6"/>
-      </tp>
-      <tp>
-        <v>2</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188924 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R6C6</stp>
-        <tr r="F6" s="6"/>
-      </tp>
-      <tp>
-        <v>4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188936 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R8C6</stp>
-        <tr r="F8" s="6"/>
-      </tp>
-      <tp>
-        <v>1</v>
+      <tp>
+        <v>-0.35699999999999998</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWEG   CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R10C6</stp>
+        <tr r="F10" s="2"/>
+      </tp>
+      <tp>
+        <v>0.4</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>CY188918 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R5C6</stp>
-        <tr r="F5" s="6"/>
-      </tp>
-      <tp>
-        <v>5</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188942 CMAN Curncy</stp>
-        <stp>TENOR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R9C6</stp>
-        <tr r="F9" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>Senior</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188930 CMAN Curncy</stp>
-        <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R7C4</stp>
-        <tr r="D7" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>Senior</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188924 CMAN Curncy</stp>
-        <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R6C4</stp>
-        <tr r="D6" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>Senior</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188918 CMAN Curncy</stp>
-        <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R5C4</stp>
-        <tr r="D5" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>GALPPL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188936 CMAN Curncy</stp>
-        <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R8C2</stp>
-        <tr r="B8" s="6"/>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R5C8</stp>
+        <tr r="H5" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>-0.36399999999999999</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWE2Z  CMPN Curncy</stp>
+        <stp>LAST PRICE</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R3C6</stp>
+        <tr r="F3" s="2"/>
       </tp>
     </main>
     <main first="bloomberg.rtd">
@@ -1621,73 +1560,285 @@
         <v>Senior</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
+        <stp>CY188942 CMAN Curncy</stp>
+        <stp>SW_SENIORITY</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R9C4</stp>
+        <tr r="D9" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALPPL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188924 CMAN Curncy</stp>
+        <stp>CDS_CORP_TKR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R6C2</stp>
+        <tr r="B6" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Senior</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188918 CMAN Curncy</stp>
+        <stp>SW_SENIORITY</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R5C4</stp>
+        <tr r="D5" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Senior</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188954 CMAN Curncy</stp>
+        <stp>SW_SENIORITY</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R11C4</stp>
+        <tr r="D11" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALPPL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188930 CMAN Curncy</stp>
+        <stp>CDS_CORP_TKR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R7C2</stp>
+        <tr r="B7" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Senior</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188948 CMAN Curncy</stp>
+        <stp>SW_SENIORITY</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R10C4</stp>
+        <tr r="D10" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALPPL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188912 CMAN Curncy</stp>
+        <stp>CDS_CORP_TKR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R4C2</stp>
+        <tr r="B4" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Senior</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188936 CMAN Curncy</stp>
+        <stp>SW_SENIORITY</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R8C4</stp>
+        <tr r="D8" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALPPL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188942 CMAN Curncy</stp>
+        <stp>CDS_CORP_TKR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R9C2</stp>
+        <tr r="B9" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Senior</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188924 CMAN Curncy</stp>
+        <stp>SW_SENIORITY</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R6C4</stp>
+        <tr r="D6" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALPPL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188918 CMAN Curncy</stp>
+        <stp>CDS_CORP_TKR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R5C2</stp>
+        <tr r="B5" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Senior</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188930 CMAN Curncy</stp>
+        <stp>SW_SENIORITY</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R7C4</stp>
+        <tr r="D7" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALPPL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188936 CMAN Curncy</stp>
+        <stp>CDS_CORP_TKR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R8C2</stp>
+        <tr r="B8" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>Senior</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
         <stp>CY188912 CMAN Curncy</stp>
         <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R4C4</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R4C4</stp>
         <tr r="D4" s="6"/>
+      </tp>
+      <tp>
+        <v>0.4</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188948 CMAN Curncy</stp>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R10C8</stp>
+        <tr r="H10" s="6"/>
+      </tp>
+      <tp>
+        <v>0.4</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188954 CMAN Curncy</stp>
+        <stp>CDS_RR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R11C8</stp>
+        <tr r="H11" s="6"/>
       </tp>
       <tp t="s">
         <v>GALPPL</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
-        <stp>CY188942 CMAN Curncy</stp>
+        <stp>CY188954 CMAN Curncy</stp>
         <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R9C2</stp>
-        <tr r="B9" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>Senior</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188942 CMAN Curncy</stp>
-        <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R9C4</stp>
-        <tr r="D9" s="6"/>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R11C2</stp>
+        <tr r="B11" s="6"/>
       </tp>
       <tp t="s">
         <v>GALPPL</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
+        <stp>CY188948 CMAN Curncy</stp>
+        <stp>CDS_CORP_TKR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R10C2</stp>
+        <tr r="B10" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>5</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188942 CMAN Curncy</stp>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R9C6</stp>
+        <tr r="F9" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>4</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188936 CMAN Curncy</stp>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R8C6</stp>
+        <tr r="F8" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>1</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188918 CMAN Curncy</stp>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R5C6</stp>
+        <tr r="F5" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>0.5</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
         <stp>CY188912 CMAN Curncy</stp>
-        <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R4C2</stp>
-        <tr r="B4" s="6"/>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R4C6</stp>
+        <tr r="F4" s="6"/>
+      </tp>
+      <tp>
+        <v>3</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188930 CMAN Curncy</stp>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R7C6</stp>
+        <tr r="F7" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>2</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188924 CMAN Curncy</stp>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R6C6</stp>
+        <tr r="F6" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>101.29900000000001</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188942 CMAN Curncy</stp>
+        <stp>CDS_FLAT_SPREAD</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R9C7</stp>
+        <tr r="G9" s="6"/>
       </tp>
       <tp t="s">
-        <v>GALPPL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188918 CMAN Curncy</stp>
-        <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R5C2</stp>
-        <tr r="B5" s="6"/>
+        <v>GALP PL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188936 CMAN Curncy</stp>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R8C3</stp>
+        <tr r="C8" s="6"/>
       </tp>
       <tp t="s">
-        <v>Senior</v>
+        <v>GALP PL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188942 CMAN Curncy</stp>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R9C3</stp>
+        <tr r="C9" s="6"/>
+      </tp>
+      <tp>
+        <v>72.61</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>CY188936 CMAN Curncy</stp>
-        <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R8C4</stp>
-        <tr r="D8" s="6"/>
+        <stp>CDS_FLAT_SPREAD</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R8C7</stp>
+        <tr r="G8" s="6"/>
       </tp>
       <tp t="s">
-        <v>GALPPL</v>
+        <v>GALP PL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188912 CMAN Curncy</stp>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R4C3</stp>
+        <tr r="C4" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>50.609999999999992</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>CY188930 CMAN Curncy</stp>
-        <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R7C2</stp>
-        <tr r="B7" s="6"/>
-      </tp>
-      <tp t="s">
-        <v>GALPPL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188924 CMAN Curncy</stp>
-        <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R6C2</stp>
-        <tr r="B6" s="6"/>
+        <stp>CDS_FLAT_SPREAD</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R7C7</stp>
+        <tr r="G7" s="6"/>
       </tp>
       <tp>
         <v>30.81</v>
@@ -1695,17 +1846,26 @@
         <stp>##V3_BDPV12</stp>
         <stp>CY188924 CMAN Curncy</stp>
         <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R6C7</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R6C7</stp>
         <tr r="G6" s="6"/>
       </tp>
       <tp>
-        <v>50.609999999999992</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188930 CMAN Curncy</stp>
+        <v>22.61</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188918 CMAN Curncy</stp>
         <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R7C7</stp>
-        <tr r="G7" s="6"/>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R5C7</stp>
+        <tr r="G5" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALP PL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188918 CMAN Curncy</stp>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R5C3</stp>
+        <tr r="C5" s="6"/>
       </tp>
       <tp>
         <v>18.48</v>
@@ -1713,260 +1873,132 @@
         <stp>##V3_BDPV12</stp>
         <stp>CY188912 CMAN Curncy</stp>
         <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R4C7</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R4C7</stp>
         <tr r="G4" s="6"/>
       </tp>
-      <tp>
-        <v>22.61</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188918 CMAN Curncy</stp>
-        <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R5C7</stp>
-        <tr r="G5" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.33429999999999999</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWE1F  CMPN Curncy</stp>
+      <tp t="s">
+        <v>GALP PL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188924 CMAN Curncy</stp>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R6C3</stp>
+        <tr r="C6" s="6"/>
+      </tp>
+      <tp t="s">
+        <v>GALP PL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188930 CMAN Curncy</stp>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R7C3</stp>
+        <tr r="C7" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>-0.35</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWEC   CMPN Curncy</stp>
         <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R16C6</stp>
-        <tr r="F16" s="2"/>
-      </tp>
-      <tp>
-        <v>72.61</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188936 CMAN Curncy</stp>
-        <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R8C7</stp>
-        <tr r="G8" s="6"/>
-      </tp>
-      <tp>
-        <v>101.29900000000001</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188942 CMAN Curncy</stp>
-        <stp>CDS_FLAT_SPREAD</stp>
-        <stp>[CDS.xlsx]CDSCurve!R9C7</stp>
-        <tr r="G9" s="6"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188948 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R10C8</stp>
-        <tr r="H10" s="6"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188954 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R11C8</stp>
-        <tr r="H11" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.30809999999999998</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWE2   CMPN Curncy</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R6C6</stp>
+        <tr r="F6" s="2"/>
+      </tp>
+      <tp>
+        <v>-0.35880000000000001</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>EUSWED   CMPN Curncy</stp>
         <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R17C6</stp>
-        <tr r="F17" s="2"/>
-      </tp>
-      <tp>
-        <v>-0.35339999999999999</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWEK   CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R14C6</stp>
-        <tr r="F14" s="2"/>
-      </tp>
-      <tp>
-        <v>-0.34960000000000002</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWE1   CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R15C6</stp>
-        <tr r="F15" s="2"/>
-      </tp>
-      <tp>
-        <v>-0.35460000000000003</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWEJ   CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R13C6</stp>
-        <tr r="F13" s="2"/>
-      </tp>
-      <tp>
-        <v>-0.3574</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWEG   CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R10C6</stp>
-        <tr r="F10" s="2"/>
-      </tp>
-      <tp>
-        <v>-0.3569</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWEH   CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R11C6</stp>
-        <tr r="F11" s="2"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188936 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R8C8</stp>
-        <tr r="H8" s="6"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188942 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R9C8</stp>
-        <tr r="H9" s="6"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188912 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R4C8</stp>
-        <tr r="H4" s="6"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188918 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R5C8</stp>
-        <tr r="H5" s="6"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188924 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R6C8</stp>
-        <tr r="H6" s="6"/>
-      </tp>
-      <tp>
-        <v>0.4</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188930 CMAN Curncy</stp>
-        <stp>CDS_RR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R7C8</stp>
-        <tr r="H7" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.35599999999999998</v>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R7C6</stp>
+        <tr r="F7" s="2"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>-0.35</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWEA   CMPN Curncy</stp>
         <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R4C6</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R4C6</stp>
         <tr r="F4" s="2"/>
       </tp>
-      <tp>
-        <v>-0.35</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWEC   CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[EoniaOIS_BBG.xlsx]EONIA!R6C6</stp>
-        <tr r="F6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>GALPPL</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188948 CMAN Curncy</stp>
-        <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R10C2</stp>
-        <tr r="B10" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.35549999999999998</v>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>-0.34799999999999998</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWEB   CMPN Curncy</stp>
         <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R5C6</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R5C6</stp>
         <tr r="F5" s="2"/>
       </tp>
-      <tp t="s">
-        <v>Senior</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188954 CMAN Curncy</stp>
-        <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R11C4</stp>
-        <tr r="D11" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.35899999999999999</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>EUSWED   CMPN Curncy</stp>
-        <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R7C6</stp>
-        <tr r="F7" s="2"/>
-      </tp>
-      <tp>
-        <v>-0.35</v>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>-0.35880000000000001</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWEE   CMPN Curncy</stp>
         <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R8C6</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R8C6</stp>
         <tr r="F8" s="2"/>
       </tp>
-      <tp t="s">
-        <v>Senior</v>
-        <stp/>
-        <stp>##V3_BDPV12</stp>
-        <stp>CY188948 CMAN Curncy</stp>
-        <stp>SW_SENIORITY</stp>
-        <stp>[CDS.xlsx]CDSCurve!R10C4</stp>
-        <tr r="D10" s="6"/>
-      </tp>
-      <tp>
-        <v>-0.35</v>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>-0.3579</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>EUSWEF   CMPN Curncy</stp>
         <stp>LAST PRICE</stp>
-        <stp>[CDS.xlsx]EONIA!R9C6</stp>
+        <stp>[CDSCurve_BBG.xlsx]EONIA!R9C6</stp>
         <tr r="F9" s="2"/>
       </tp>
+    </main>
+    <main first="bloomberg.rtd">
       <tp t="s">
-        <v>GALPPL</v>
+        <v>GALP PL</v>
         <stp/>
         <stp>##V3_BDPV12</stp>
         <stp>CY188954 CMAN Curncy</stp>
-        <stp>CDS_CORP_TKR</stp>
-        <stp>[CDS.xlsx]CDSCurve!R11C2</stp>
-        <tr r="B11" s="6"/>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R11C3</stp>
+        <tr r="C11" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp t="s">
+        <v>GALP PL</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188948 CMAN Curncy</stp>
+        <stp>PRIMARY_EQUITY_TICKER</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R10C3</stp>
+        <tr r="C10" s="6"/>
+      </tp>
+    </main>
+    <main first="bloomberg.rtd">
+      <tp>
+        <v>7</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188948 CMAN Curncy</stp>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R10C6</stp>
+        <tr r="F10" s="6"/>
+      </tp>
+      <tp>
+        <v>10</v>
+        <stp/>
+        <stp>##V3_BDPV12</stp>
+        <stp>CY188954 CMAN Curncy</stp>
+        <stp>TENOR</stp>
+        <stp>[CDSCurve_BBG.xlsx]CDSCurve!R11C6</stp>
+        <tr r="F11" s="6"/>
       </tp>
     </main>
   </volType>
@@ -2273,7 +2305,7 @@
   <dimension ref="B1:AG35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.5"/>
@@ -2296,7 +2328,7 @@
       </c>
       <c r="C2" s="10">
         <f ca="1">TODAY()</f>
-        <v>43536</v>
+        <v>43538</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="25" t="s">
@@ -2325,14 +2357,14 @@
       </c>
       <c r="F3" s="20">
         <f>_xll.BDP(E3, "LAST PRICE")/100</f>
-        <v>-3.6099999999999999E-3</v>
+        <v>-3.64E-3</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G3,F3,$C$6)</f>
-        <v>obj_0007b#0001</v>
+        <v>obj_00083#0006</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -2343,14 +2375,14 @@
       </c>
       <c r="F4" s="20">
         <f>_xll.BDP(E4, "LAST PRICE")/100</f>
-        <v>-3.5599999999999998E-3</v>
+        <v>-3.4999999999999996E-3</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G4,F4,$C$6)</f>
-        <v>obj_0007f#0001</v>
+        <v>obj_00086#0006</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -2361,14 +2393,14 @@
       </c>
       <c r="F5" s="20">
         <f>_xll.BDP(E5, "LAST PRICE")/100</f>
-        <v>-3.555E-3</v>
+        <v>-3.4799999999999996E-3</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G5,F5,$C$6)</f>
-        <v>obj_0006d#0001</v>
+        <v>obj_0007e#0006</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -2377,7 +2409,7 @@
       </c>
       <c r="C6" s="16" t="str">
         <f>_xll.qlEonia()</f>
-        <v>obj_00003#0011</v>
+        <v>obj_00073#0006</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>54</v>
@@ -2391,7 +2423,7 @@
       </c>
       <c r="H6" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G6,F6,$C$6)</f>
-        <v>obj_00073#0000</v>
+        <v>obj_00080#0006</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -2406,14 +2438,14 @@
       </c>
       <c r="F7" s="20">
         <f>_xll.BDP(E7, "LAST PRICE")/100</f>
-        <v>-3.5899999999999999E-3</v>
+        <v>-3.588E-3</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G7,F7,$C$6)</f>
-        <v>obj_0007a#0001</v>
+        <v>obj_00090#0007</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -2428,14 +2460,14 @@
       </c>
       <c r="F8" s="20">
         <f>_xll.BDP(E8, "LAST PRICE")/100</f>
-        <v>-3.4999999999999996E-3</v>
+        <v>-3.588E-3</v>
       </c>
       <c r="G8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="H8" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G8,F8,$C$6)</f>
-        <v>obj_0007e#0001</v>
+        <v>obj_0008f#0005</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -2450,14 +2482,14 @@
       </c>
       <c r="F9" s="20">
         <f>_xll.BDP(E9, "LAST PRICE")/100</f>
-        <v>-3.4999999999999996E-3</v>
+        <v>-3.5790000000000001E-3</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>7</v>
       </c>
       <c r="H9" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G9,F9,$C$6)</f>
-        <v>obj_00080#0001</v>
+        <v>obj_0007b#0008</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -2470,14 +2502,14 @@
       </c>
       <c r="F10" s="20">
         <f>_xll.BDP(E10, "LAST PRICE")/100</f>
-        <v>-3.5739999999999999E-3</v>
+        <v>-3.5699999999999998E-3</v>
       </c>
       <c r="G10" s="18" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G10,F10,$C$6)</f>
-        <v>obj_00071#0001</v>
+        <v>obj_0007f#0006</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -2490,14 +2522,14 @@
       </c>
       <c r="F11" s="20">
         <f>_xll.BDP(E11, "LAST PRICE")/100</f>
-        <v>-3.5690000000000001E-3</v>
+        <v>-3.5799999999999998E-3</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="H11" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G11,F11,$C$6)</f>
-        <v>obj_00088#0002</v>
+        <v>obj_00082#0006</v>
       </c>
     </row>
     <row r="12" spans="2:8">
@@ -2506,21 +2538,21 @@
       </c>
       <c r="C12" s="14" t="str">
         <f>_xll.qlPiecewiseYieldCurve(,0,C7,H3:H35,C9)</f>
-        <v>obj_00090#0005</v>
+        <v>obj_00095#0064</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>60</v>
       </c>
       <c r="F12" s="20">
         <f>_xll.BDP(E12, "LAST PRICE")/100</f>
-        <v>-3.5570000000000003E-3</v>
+        <v>-3.5699999999999998E-3</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="H12" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G12,F12,$C$6)</f>
-        <v>obj_0008e#0003</v>
+        <v>obj_00085#0006</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -2536,14 +2568,14 @@
       </c>
       <c r="F13" s="20">
         <f>_xll.BDP(E13, "LAST PRICE")/100</f>
-        <v>-3.5460000000000001E-3</v>
+        <v>-3.5499999999999998E-3</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H13" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G13,F13,$C$6)</f>
-        <v>obj_0006e#0002</v>
+        <v>obj_00075#0007</v>
       </c>
     </row>
     <row r="14" spans="2:8">
@@ -2552,14 +2584,14 @@
       </c>
       <c r="F14" s="20">
         <f>_xll.BDP(E14, "LAST PRICE")/100</f>
-        <v>-3.5339999999999998E-3</v>
+        <v>-3.5349999999999999E-3</v>
       </c>
       <c r="G14" s="18" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G14,F14,$C$6)</f>
-        <v>obj_0008c#0003</v>
+        <v>obj_00079#0006</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -2568,14 +2600,14 @@
       </c>
       <c r="F15" s="20">
         <f>_xll.BDP(E15, "LAST PRICE")/100</f>
-        <v>-3.4960000000000004E-3</v>
+        <v>-3.5199999999999997E-3</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>13</v>
       </c>
       <c r="H15" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G15,F15,$C$6)</f>
-        <v>obj_00079#0002</v>
+        <v>obj_00093#0007</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -2584,14 +2616,14 @@
       </c>
       <c r="F16" s="20">
         <f>_xll.BDP(E16, "LAST PRICE")/100</f>
-        <v>-3.3430000000000001E-3</v>
+        <v>-3.3639999999999998E-3</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G16,F16,$C$6)</f>
-        <v>obj_00086#0002</v>
+        <v>obj_00078#0010</v>
       </c>
     </row>
     <row r="17" spans="5:8">
@@ -2600,14 +2632,14 @@
       </c>
       <c r="F17" s="20">
         <f>_xll.BDP(E17, "LAST PRICE")/100</f>
-        <v>-3.081E-3</v>
+        <v>-3.107E-3</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G17,F17,$C$6)</f>
-        <v>obj_00081#0003</v>
+        <v>obj_00087#0009</v>
       </c>
     </row>
     <row r="18" spans="5:8">
@@ -2616,14 +2648,14 @@
       </c>
       <c r="F18" s="20">
         <f>_xll.BDP(E18, "LAST PRICE")/100</f>
-        <v>-2.7529999999999998E-3</v>
+        <v>-2.7900000000000004E-3</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G18,F18,$C$6)</f>
-        <v>obj_00084#0000</v>
+        <v>obj_0007d#0006</v>
       </c>
     </row>
     <row r="19" spans="5:8">
@@ -2632,14 +2664,14 @@
       </c>
       <c r="F19" s="20">
         <f>_xll.BDP(E19, "LAST PRICE")/100</f>
-        <v>-2.382E-3</v>
+        <v>-2.4250000000000001E-3</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G19,F19,$C$6)</f>
-        <v>obj_00089#0003</v>
+        <v>obj_0008b#0014</v>
       </c>
     </row>
     <row r="20" spans="5:8">
@@ -2648,14 +2680,14 @@
       </c>
       <c r="F20" s="20">
         <f>_xll.BDP(E20, "LAST PRICE")/100</f>
-        <v>-1.578E-3</v>
+        <v>-1.6050000000000001E-3</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H20" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G20,F20,$C$6)</f>
-        <v>obj_0007d#0004</v>
+        <v>obj_00084#0009</v>
       </c>
     </row>
     <row r="21" spans="5:8">
@@ -2664,14 +2696,14 @@
       </c>
       <c r="F21" s="20">
         <f>_xll.BDP(E21, "LAST PRICE")/100</f>
-        <v>-7.049999999999999E-4</v>
+        <v>-7.2999999999999996E-4</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G21,F21,$C$6)</f>
-        <v>obj_0006f#0004</v>
+        <v>obj_00074#0009</v>
       </c>
     </row>
     <row r="22" spans="5:8">
@@ -2680,14 +2712,14 @@
       </c>
       <c r="F22" s="20">
         <f>_xll.BDP(E22, "LAST PRICE")/100</f>
-        <v>2.5700000000000001E-4</v>
+        <v>2.1499999999999999E-4</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H22" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G22,F22,$C$6)</f>
-        <v>obj_00074#0005</v>
+        <v>obj_00077#0010</v>
       </c>
     </row>
     <row r="23" spans="5:8">
@@ -2696,14 +2728,14 @@
       </c>
       <c r="F23" s="20">
         <f>_xll.BDP(E23, "LAST PRICE")/100</f>
-        <v>1.23E-3</v>
+        <v>1.2049999999999999E-3</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>21</v>
       </c>
       <c r="H23" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G23,F23,$C$6)</f>
-        <v>obj_00078#0003</v>
+        <v>obj_00091#0014</v>
       </c>
     </row>
     <row r="24" spans="5:8">
@@ -2712,14 +2744,14 @@
       </c>
       <c r="F24" s="20">
         <f>_xll.BDP(E24, "LAST PRICE")/100</f>
-        <v>2.225E-3</v>
+        <v>2.2079999999999999E-3</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>22</v>
       </c>
       <c r="H24" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G24,F24,$C$6)</f>
-        <v>obj_0007c#0004</v>
+        <v>obj_00092#0013</v>
       </c>
     </row>
     <row r="25" spans="5:8">
@@ -2728,14 +2760,14 @@
       </c>
       <c r="F25" s="20">
         <f>_xll.BDP(E25, "LAST PRICE")/100</f>
-        <v>3.2069999999999998E-3</v>
+        <v>3.202E-3</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>23</v>
       </c>
       <c r="H25" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G25,F25,$C$6)</f>
-        <v>obj_00082#0005</v>
+        <v>obj_0007a#0016</v>
       </c>
     </row>
     <row r="26" spans="5:8">
@@ -2744,14 +2776,14 @@
       </c>
       <c r="F26" s="20">
         <f>_xll.BDP(E26, "LAST PRICE")/100</f>
-        <v>4.1549999999999998E-3</v>
+        <v>4.1330000000000004E-3</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G26,F26,$C$6)</f>
-        <v>obj_00072#0004</v>
+        <v>obj_0007c#0018</v>
       </c>
     </row>
     <row r="27" spans="5:8">
@@ -2760,14 +2792,14 @@
       </c>
       <c r="F27" s="20">
         <f>_xll.BDP(E27, "LAST PRICE")/100</f>
-        <v>5.0349999999999995E-3</v>
+        <v>5.0270000000000002E-3</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>25</v>
       </c>
       <c r="H27" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G27,F27,$C$6)</f>
-        <v>obj_0008a#0004</v>
+        <v>obj_00081#0013</v>
       </c>
     </row>
     <row r="28" spans="5:8">
@@ -2776,14 +2808,14 @@
       </c>
       <c r="F28" s="20">
         <f>_xll.BDP(E28, "LAST PRICE")/100</f>
-        <v>5.875E-3</v>
+        <v>5.8399999999999997E-3</v>
       </c>
       <c r="G28" s="18" t="s">
         <v>26</v>
       </c>
       <c r="H28" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G28,F28,$C$6)</f>
-        <v>obj_0008f#0004</v>
+        <v>obj_0008e#0011</v>
       </c>
     </row>
     <row r="29" spans="5:8">
@@ -2792,14 +2824,14 @@
       </c>
       <c r="F29" s="20">
         <f>_xll.BDP(E29, "LAST PRICE")/100</f>
-        <v>7.8100000000000001E-3</v>
+        <v>7.7800000000000005E-3</v>
       </c>
       <c r="G29" s="18" t="s">
         <v>27</v>
       </c>
       <c r="H29" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G29,F29,$C$6)</f>
-        <v>obj_00070#0005</v>
+        <v>obj_00076#0012</v>
       </c>
     </row>
     <row r="30" spans="5:8">
@@ -2808,14 +2840,14 @@
       </c>
       <c r="F30" s="20">
         <f>_xll.BDP(E30, "LAST PRICE")/100</f>
-        <v>9.6249999999999999E-3</v>
+        <v>9.6120000000000008E-3</v>
       </c>
       <c r="G30" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H30" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G30,F30,$C$6)</f>
-        <v>obj_0008d#0005</v>
+        <v>obj_0008d#0011</v>
       </c>
     </row>
     <row r="31" spans="5:8">
@@ -2824,14 +2856,14 @@
       </c>
       <c r="F31" s="20">
         <f>_xll.BDP(E31, "LAST PRICE")/100</f>
-        <v>1.0347E-2</v>
+        <v>1.0335E-2</v>
       </c>
       <c r="G31" s="18" t="s">
         <v>29</v>
       </c>
       <c r="H31" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G31,F31,$C$6)</f>
-        <v>obj_00077#0005</v>
+        <v>obj_00094#0016</v>
       </c>
     </row>
     <row r="32" spans="5:8">
@@ -2840,14 +2872,14 @@
       </c>
       <c r="F32" s="20">
         <f>_xll.BDP(E32, "LAST PRICE")/100</f>
-        <v>1.0629999999999999E-2</v>
+        <v>1.0625000000000001E-2</v>
       </c>
       <c r="G32" s="18" t="s">
         <v>30</v>
       </c>
       <c r="H32" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G32,F32,$C$6)</f>
-        <v>obj_00087#0005</v>
+        <v>obj_0008a#0012</v>
       </c>
     </row>
     <row r="33" spans="5:33">
@@ -2856,14 +2888,14 @@
       </c>
       <c r="F33" s="20">
         <f>_xll.BDP(E33, "LAST PRICE")/100</f>
-        <v>1.0697000000000002E-2</v>
+        <v>1.0688999999999999E-2</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H33" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G33,F33,$C$6)</f>
-        <v>obj_00083#0004</v>
+        <v>obj_00088#0012</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -2896,14 +2928,14 @@
       </c>
       <c r="F34" s="20">
         <f>_xll.BDP(E34, "LAST PRICE")/100</f>
-        <v>1.0695E-2</v>
+        <v>1.0708000000000001E-2</v>
       </c>
       <c r="G34" s="18" t="s">
         <v>32</v>
       </c>
       <c r="H34" s="21" t="str">
         <f>_xll.qlOISRateHelper(,2,G34,F34,$C$6)</f>
-        <v>obj_00085#0004</v>
+        <v>obj_00089#0013</v>
       </c>
     </row>
     <row r="35" spans="5:33">
@@ -2912,14 +2944,14 @@
       </c>
       <c r="F35" s="22">
         <f>_xll.BDP(E35, "LAST PRICE")/100</f>
-        <v>1.0615000000000001E-2</v>
+        <v>1.0618000000000001E-2</v>
       </c>
       <c r="G35" s="23" t="s">
         <v>33</v>
       </c>
       <c r="H35" s="24" t="str">
         <f>_xll.qlOISRateHelper(,2,G35,F35,$C$6)</f>
-        <v>obj_0008b#0003</v>
+        <v>obj_0008c#0013</v>
       </c>
     </row>
   </sheetData>
@@ -2935,7 +2967,7 @@
   <dimension ref="B2:O30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.53125" defaultRowHeight="12.75"/>
@@ -3025,15 +3057,15 @@
       </c>
       <c r="J4" s="49" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G4/10000,$F4,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H4,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000e6#0055</v>
+        <v>obj_00096#0064</v>
       </c>
       <c r="L4" s="39" t="str">
         <f>_xll.qlPiecewiseHazardRateCurve(,J4:J11,EONIA!$C$9,EONIA!$C$7,"BACKWARDFLAT")</f>
-        <v>obj_000ed#0037</v>
+        <v>obj_0009e#0064</v>
       </c>
       <c r="N4" s="54">
         <f ca="1">Today</f>
-        <v>43536</v>
+        <v>43538</v>
       </c>
       <c r="O4" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N4,TRUE)</f>
@@ -3070,15 +3102,15 @@
       </c>
       <c r="J5" s="49" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G5/10000,$F5,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H5,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000e7#0019</v>
+        <v>obj_0009b#0064</v>
       </c>
       <c r="N5" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N4,"6M","Unadjusted")</f>
-        <v>43720</v>
+        <v>43722</v>
       </c>
       <c r="O5" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N5,TRUE)</f>
-        <v>1.573718981596306E-3</v>
+        <v>1.5737299764581048E-3</v>
       </c>
     </row>
     <row r="6" spans="2:15">
@@ -3111,15 +3143,15 @@
       </c>
       <c r="J6" s="49" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G6/10000,$F6,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H6,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000e9#0019</v>
+        <v>obj_0009a#0064</v>
       </c>
       <c r="N6" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N5,"6M","Unadjusted")</f>
-        <v>43902</v>
+        <v>43904</v>
       </c>
       <c r="O6" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N6,TRUE)</f>
-        <v>3.8073759522273543E-3</v>
+        <v>3.8114994491019738E-3</v>
       </c>
     </row>
     <row r="7" spans="2:15">
@@ -3152,15 +3184,15 @@
       </c>
       <c r="J7" s="49" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G7/10000,$F7,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H7,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000eb#0019</v>
+        <v>obj_0009c#0064</v>
       </c>
       <c r="N7" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N6,"6M","Unadjusted")</f>
-        <v>44086</v>
+        <v>44088</v>
       </c>
       <c r="O7" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N7,TRUE)</f>
-        <v>7.0849892837789863E-3</v>
+        <v>7.0965306248420568E-3</v>
       </c>
     </row>
     <row r="8" spans="2:15">
@@ -3193,15 +3225,15 @@
       </c>
       <c r="J8" s="49" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G8/10000,$F8,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H8,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000ec#0019</v>
+        <v>obj_0009d#0064</v>
       </c>
       <c r="N8" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N7,"6M","Unadjusted")</f>
-        <v>44267</v>
+        <v>44269</v>
       </c>
       <c r="O8" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N8,TRUE)</f>
-        <v>1.0342874732126695E-2</v>
+        <v>1.0350606638163229E-2</v>
       </c>
     </row>
     <row r="9" spans="2:15">
@@ -3234,15 +3266,15 @@
       </c>
       <c r="J9" s="49" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G9/10000,$F9,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H9,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000ef#0004</v>
+        <v>obj_00099#0064</v>
       </c>
       <c r="N9" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N8,"6M","Unadjusted")</f>
-        <v>44451</v>
+        <v>44453</v>
       </c>
       <c r="O9" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N9,TRUE)</f>
-        <v>1.7793822412378035E-2</v>
+        <v>1.7839794530003505E-2</v>
       </c>
     </row>
     <row r="10" spans="2:15">
@@ -3275,15 +3307,15 @@
       </c>
       <c r="J10" s="49" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G10/10000,$F10,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H10,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000e8#0019</v>
+        <v>obj_00098#0064</v>
       </c>
       <c r="N10" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N9,"6M","Unadjusted")</f>
-        <v>44632</v>
+        <v>44634</v>
       </c>
       <c r="O10" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N10,TRUE)</f>
-        <v>2.5300914895276305E-2</v>
+        <v>2.5337212320292735E-2</v>
       </c>
     </row>
     <row r="11" spans="2:15">
@@ -3317,75 +3349,75 @@
       <c r="I11" s="31"/>
       <c r="J11" s="50" t="str">
         <f>_xll.qlSpreadCdsHelper(,$G11/10000,$F11,1,"TARGET","Quarterly","Modified Following","OldCDS",EONIA!$C$9,$H11,EONIA!$C$12,TRUE,TRUE,TRUE)</f>
-        <v>obj_000ea#0019</v>
+        <v>obj_00097#0064</v>
       </c>
       <c r="N11" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N10,"6M","Unadjusted")</f>
-        <v>44816</v>
+        <v>44818</v>
       </c>
       <c r="O11" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N11,TRUE)</f>
-        <v>3.6775227413824774E-2</v>
+        <v>3.6844590101280383E-2</v>
       </c>
     </row>
     <row r="12" spans="2:15">
       <c r="N12" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N11,"6M","Unadjusted")</f>
-        <v>44997</v>
+        <v>44999</v>
       </c>
       <c r="O12" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N12,TRUE)</f>
-        <v>4.8125340820214357E-2</v>
+        <v>4.8183125606738875E-2</v>
       </c>
     </row>
     <row r="13" spans="2:15">
       <c r="N13" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N12,"6M","Unadjusted")</f>
-        <v>45181</v>
+        <v>45183</v>
       </c>
       <c r="O13" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N13,TRUE)</f>
-        <v>6.5797133691153253E-2</v>
+        <v>6.5910143697596846E-2</v>
       </c>
     </row>
     <row r="14" spans="2:15">
       <c r="N14" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N13,"6M","Unadjusted")</f>
-        <v>45363</v>
+        <v>45365</v>
       </c>
       <c r="O14" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N14,TRUE)</f>
-        <v>8.3229855299607802E-2</v>
+        <v>8.3326343487255539E-2</v>
       </c>
     </row>
     <row r="15" spans="2:15">
       <c r="N15" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N14,"6M","Unadjusted")</f>
-        <v>45547</v>
+        <v>45549</v>
       </c>
       <c r="O15" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N15,TRUE)</f>
-        <v>0.10132218150414107</v>
+        <v>0.101416214903298</v>
       </c>
     </row>
     <row r="16" spans="2:15">
       <c r="N16" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N15,"6M","Unadjusted")</f>
-        <v>45728</v>
+        <v>45730</v>
       </c>
       <c r="O16" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N16,TRUE)</f>
-        <v>0.11880612479985797</v>
+        <v>0.11888919955928201</v>
       </c>
     </row>
     <row r="17" spans="2:15">
       <c r="N17" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N16,"6M","Unadjusted")</f>
-        <v>45912</v>
+        <v>45914</v>
       </c>
       <c r="O17" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N17,TRUE)</f>
-        <v>0.13623123794060188</v>
+        <v>0.13630357285003014</v>
       </c>
     </row>
     <row r="18" spans="2:15">
@@ -3395,11 +3427,11 @@
       <c r="C18" s="41"/>
       <c r="N18" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N17,"6M","Unadjusted")</f>
-        <v>46093</v>
+        <v>46095</v>
       </c>
       <c r="O18" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N18,TRUE)</f>
-        <v>0.15303601908200692</v>
+        <v>0.1530981719395248</v>
       </c>
     </row>
     <row r="19" spans="2:15">
@@ -3411,11 +3443,11 @@
       </c>
       <c r="N19" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N18,"6M","Unadjusted")</f>
-        <v>46277</v>
+        <v>46279</v>
       </c>
       <c r="O19" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N19,TRUE)</f>
-        <v>0.1698018628730309</v>
+        <v>0.16985692629706917</v>
       </c>
     </row>
     <row r="20" spans="2:15">
@@ -3427,11 +3459,11 @@
       </c>
       <c r="N20" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N19,"6M","Unadjusted")</f>
-        <v>46458</v>
+        <v>46460</v>
       </c>
       <c r="O20" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N20,TRUE)</f>
-        <v>0.18597127638813649</v>
+        <v>0.18601951031072617</v>
       </c>
     </row>
     <row r="21" spans="2:15">
@@ -3440,15 +3472,15 @@
       </c>
       <c r="C21" s="37" t="str">
         <f ca="1">_xll.qlSchedule(,Today+1,_xll.qlCalendarAdvance("TARGET",Today,C20),"3M","TARGET","Unadjusted","Unadjusted","OldCDS")</f>
-        <v>obj_000ee#0008</v>
+        <v>obj_00042#2308</v>
       </c>
       <c r="N21" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N20,"6M","Unadjusted")</f>
-        <v>46642</v>
+        <v>46644</v>
       </c>
       <c r="O21" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N21,TRUE)</f>
-        <v>0.20208592851526141</v>
+        <v>0.20212747093103078</v>
       </c>
     </row>
     <row r="22" spans="2:15">
@@ -3460,11 +3492,11 @@
       </c>
       <c r="N22" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N21,"6M","Unadjusted")</f>
-        <v>46824</v>
+        <v>46826</v>
       </c>
       <c r="O22" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N22,TRUE)</f>
-        <v>0.21771157272115249</v>
+        <v>0.21774673838292136</v>
       </c>
     </row>
     <row r="23" spans="2:15">
@@ -3476,11 +3508,11 @@
       </c>
       <c r="N23" s="55">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N22,"6M","Unadjusted")</f>
-        <v>47008</v>
+        <v>47010</v>
       </c>
       <c r="O23" s="33">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N23,TRUE)</f>
-        <v>0.23319788850217293</v>
+        <v>0.23322684496144974</v>
       </c>
     </row>
     <row r="24" spans="2:15">
@@ -3489,15 +3521,15 @@
       </c>
       <c r="C24" s="37" t="str">
         <f ca="1">_xll.qlCreditDefaultSwap(,"BUYER",1000000,A25,C23/10000,C21,"Modified Following",EONIA!C9,TRUE,TRUE,Today+1,,TRUE)</f>
-        <v>obj_000f0#0009</v>
+        <v>obj_00043#2308</v>
       </c>
       <c r="N24" s="56">
         <f ca="1">_xll.qlCalendarAdvance("TARGET",N23,"6M","Unadjusted")</f>
-        <v>47189</v>
+        <v>47191</v>
       </c>
       <c r="O24" s="32">
         <f ca="1">_xll.qlDefaultTSDefaultProbability($L$4,N24,TRUE)</f>
-        <v>0.24813256478074452</v>
+        <v>0.24815563968408372</v>
       </c>
     </row>
     <row r="25" spans="2:15">
@@ -3506,7 +3538,7 @@
       </c>
       <c r="C25" s="37" t="str">
         <f>_xll.qlMidPointCdsEngine(,L4,H11,EONIA!C12)</f>
-        <v>obj_000f1#0013</v>
+        <v>obj_0009f#0064</v>
       </c>
     </row>
     <row r="26" spans="2:15">
@@ -3522,7 +3554,7 @@
       </c>
       <c r="C27" s="38">
         <f ca="1">_xll.qlInstrumentNPV(C24,C25)</f>
-        <v>-1833.4313678622784</v>
+        <v>-1831.6886442634495</v>
       </c>
     </row>
     <row r="28" spans="2:15">
@@ -3547,9 +3579,9 @@
       <c r="B30" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="39" t="e">
+      <c r="C30" s="39">
         <f ca="1">_xll.qlCdsFairUpfront(C24,C25)</f>
-        <v>#NUM!</v>
+        <v>-1.8316117191184275E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>